<commit_message>
Cambio modulo de flash
Cambio modulo de flash
</commit_message>
<xml_diff>
--- a/Documentos/Configuración del Linker File.xlsx
+++ b/Documentos/Configuración del Linker File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2708d86aa79f336/Documentos/Git/pic32mmBoot/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{7754BBE6-71FB-49C0-88F8-31E2ED0AEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0AF3952-B372-4ED5-ADA0-A5F274C97AE2}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{7754BBE6-71FB-49C0-88F8-31E2ED0AEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0630674-B54D-4296-8953-61E020D8E58E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="13020" xr2:uid="{A2A9E1D7-DA62-45E2-AF5C-44894F864DBD}"/>
+    <workbookView xWindow="-19320" yWindow="6030" windowWidth="19440" windowHeight="15600" xr2:uid="{A2A9E1D7-DA62-45E2-AF5C-44894F864DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>ORIGIN = 0x9D000000, LENGTH = 0x5000</t>
   </si>
   <si>
-    <t>Inicio Program1 + BooLen</t>
-  </si>
-  <si>
     <t>Inicio Program1 + BootLen + 0x1000</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>ORIGIN = 0x9D006490, LENGTH = 0x39B70</t>
+  </si>
+  <si>
+    <t>Inicio Program1 + BootLen</t>
   </si>
 </sst>
 </file>
@@ -359,10 +359,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -684,35 +680,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259B4523-2ADC-4EBE-8D26-57DEBCA310C8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" customWidth="1"/>
-    <col min="2" max="2" width="37.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -727,7 +723,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -742,7 +738,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -757,7 +753,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -772,7 +768,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -787,7 +783,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -804,7 +800,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -821,7 +817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -838,7 +834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -855,7 +851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -866,10 +862,10 @@
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -880,10 +876,10 @@
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
@@ -894,10 +890,10 @@
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -908,10 +904,10 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -922,10 +918,10 @@
         <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -936,10 +932,10 @@
         <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -950,10 +946,10 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
@@ -964,23 +960,23 @@
         <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7" t="s">
         <v>1</v>
@@ -995,7 +991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>5</v>
       </c>
@@ -1005,12 +1001,12 @@
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>62</v>
+      <c r="D26" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
@@ -1025,7 +1021,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>9</v>
       </c>
@@ -1036,11 +1032,11 @@
         <v>8</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -1051,11 +1047,11 @@
         <v>10</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>15</v>
       </c>
@@ -1066,13 +1062,13 @@
         <v>53</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>13</v>
       </c>
@@ -1083,13 +1079,13 @@
         <v>23</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
@@ -1100,13 +1096,13 @@
         <v>23</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1113,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Debug y correcciones de flash
Se agrega una salida de mensajes de debug por serial y se corrije la implementación de funciones de escitura en el flash interno
</commit_message>
<xml_diff>
--- a/Documentos/Configuración del Linker File.xlsx
+++ b/Documentos/Configuración del Linker File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2708d86aa79f336/Documentos/Git/pic32mmBoot/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{7754BBE6-71FB-49C0-88F8-31E2ED0AEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0630674-B54D-4296-8953-61E020D8E58E}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{7754BBE6-71FB-49C0-88F8-31E2ED0AEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0B24975-0303-4944-BFB8-DB5D625103B2}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="6030" windowWidth="19440" windowHeight="15600" xr2:uid="{A2A9E1D7-DA62-45E2-AF5C-44894F864DBD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A2A9E1D7-DA62-45E2-AF5C-44894F864DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>PIC32MX795F512L</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Inicio Program1 +BootLen + 0x1000 + 0X380</t>
   </si>
   <si>
-    <t>Inicio Program1 + BootLen + 0x1000 + 0X380</t>
-  </si>
-  <si>
     <t>Mueve el origen BootLen + 0x1000 + 0x490 y se lo resta al tamao de memoria (0x80000)</t>
   </si>
   <si>
@@ -243,6 +240,15 @@
   </si>
   <si>
     <t>Inicio Program1 + BootLen</t>
+  </si>
+  <si>
+    <t>Bootloader len:</t>
+  </si>
+  <si>
+    <t>0x5000</t>
+  </si>
+  <si>
+    <t>Inicio Program1 + BootLen + 0x1000 + 0X480</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -344,6 +350,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,6 +366,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,444 +689,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259B4523-2ADC-4EBE-8D26-57DEBCA310C8}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="34.7265625" customWidth="1"/>
+    <col min="3" max="3" width="33.81640625" customWidth="1"/>
+    <col min="4" max="4" width="72.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
       </c>
       <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
       <c r="D21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="E32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="C33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Todo Ok pero se pisa el boot con el pgm
Todo Ok pero se pisa el boot con el pgm
</commit_message>
<xml_diff>
--- a/Documentos/Configuración del Linker File.xlsx
+++ b/Documentos/Configuración del Linker File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2708d86aa79f336/Documentos/Git/pic32mmBoot/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{7754BBE6-71FB-49C0-88F8-31E2ED0AEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0B24975-0303-4944-BFB8-DB5D625103B2}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{7754BBE6-71FB-49C0-88F8-31E2ED0AEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{861EA799-95F6-4EB7-9684-5FF8FA2AB0C8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A2A9E1D7-DA62-45E2-AF5C-44894F864DBD}"/>
+    <workbookView xWindow="-19320" yWindow="6030" windowWidth="19440" windowHeight="15600" xr2:uid="{A2A9E1D7-DA62-45E2-AF5C-44894F864DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>PIC32MX795F512L</t>
   </si>
@@ -194,9 +194,6 @@
     <t>ORIGIN = 0x9FC00490, LENGTH = 0x760</t>
   </si>
   <si>
-    <t>20K - 0x5000</t>
-  </si>
-  <si>
     <t>ORIGIN = 0x9D000000, LENGTH = 0x5000</t>
   </si>
   <si>
@@ -218,37 +215,31 @@
     <t>Inicio Program1 + BootLen + 0x1000 y length 0x490</t>
   </si>
   <si>
-    <t>0x9D005000</t>
-  </si>
-  <si>
-    <t>0x9D006380</t>
-  </si>
-  <si>
-    <t>0x9D006480</t>
-  </si>
-  <si>
-    <t>ORIGIN = 0x9D005000, LENGTH = 0x0</t>
-  </si>
-  <si>
-    <t>ORIGIN = 0x9D005000, LENGTH = 0x1000</t>
-  </si>
-  <si>
     <t>ORIGIN = 0x9D006000, LENGTH = 0x490</t>
   </si>
   <si>
-    <t>ORIGIN = 0x9D006490, LENGTH = 0x39B70</t>
-  </si>
-  <si>
     <t>Inicio Program1 + BootLen</t>
   </si>
   <si>
     <t>Bootloader len:</t>
   </si>
   <si>
-    <t>0x5000</t>
-  </si>
-  <si>
     <t>Inicio Program1 + BootLen + 0x1000 + 0X480</t>
+  </si>
+  <si>
+    <t>0x9D007000</t>
+  </si>
+  <si>
+    <t>0x9D007380</t>
+  </si>
+  <si>
+    <t>0x9D007480</t>
+  </si>
+  <si>
+    <t>ORIGIN = 0x9D007490, LENGTH = 0x38B70</t>
+  </si>
+  <si>
+    <t>0x6000 - 24K</t>
   </si>
 </sst>
 </file>
@@ -311,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -334,11 +325,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -348,9 +419,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +444,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,40 +765,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259B4523-2ADC-4EBE-8D26-57DEBCA310C8}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
-    <col min="3" max="3" width="33.81640625" customWidth="1"/>
-    <col min="4" max="4" width="72.54296875" customWidth="1"/>
-    <col min="5" max="5" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -739,7 +829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -754,7 +844,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -769,7 +859,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -784,7 +874,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -799,7 +889,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -816,7 +906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -833,7 +923,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -850,7 +940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -867,138 +957,161 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="D22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="7" t="s">
         <v>1</v>
@@ -1013,7 +1126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>5</v>
       </c>
@@ -1023,12 +1136,12 @@
       <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>60</v>
+      <c r="D27" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
@@ -1038,12 +1151,12 @@
       <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>27</v>
+      <c r="D28" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>9</v>
       </c>
@@ -1053,12 +1166,12 @@
       <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>61</v>
+      <c r="D29" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>11</v>
       </c>
@@ -1068,46 +1181,46 @@
       <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>62</v>
+      <c r="D30" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="10" t="s">
+      <c r="C31" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>66</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>63</v>
+      <c r="D32" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>18</v>
       </c>
@@ -1117,14 +1230,14 @@
       <c r="C33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>64</v>
+      <c r="D33" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
@@ -1134,8 +1247,8 @@
       <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>65</v>
+      <c r="D34" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>25</v>

</xml_diff>